<commit_message>
Update ProjektbeglBericht & Rechnungsstellung
Rechnungsstellung noch hübsch machen
</commit_message>
<xml_diff>
--- a/Dokumentationen/Projektbegleitender Bericht.xlsx
+++ b/Dokumentationen/Projektbegleitender Bericht.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Überarbeitung Pflichtenheft, Anwender- &amp; Admindoku</t>
+  </si>
+  <si>
+    <t>Rechnungsstellung</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Total Softwarewartung</t>
   </si>
 </sst>
 </file>
@@ -167,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -184,11 +193,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -201,6 +219,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -515,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -896,7 +917,9 @@
         <v>42874</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10">
+        <v>0.5</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10">
         <v>1</v>
@@ -958,6 +981,50 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="11">
+        <v>42894</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="14">
+        <v>2</v>
+      </c>
+      <c r="E37" s="14">
+        <v>1</v>
+      </c>
+      <c r="F37" s="14">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>